<commit_message>
Implements cam-centric-cord-converter in an AprilTagOMeter
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
+++ b/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360A5670-EDE0-6D47-B337-1AC396332D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE7F138-709A-844E-BEA2-0C2025F8793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
   </bookViews>
   <sheets>
     <sheet name="id1 - Straight On (Angle Cxled)" sheetId="1" r:id="rId1"/>
     <sheet name="id2 - Pointing" sheetId="2" r:id="rId2"/>
+    <sheet name="ALLid - Const. Angle" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,11 +39,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Location</t>
   </si>
   <si>
+    <t>Measured X</t>
+  </si>
+  <si>
+    <t>Measured Y</t>
+  </si>
+  <si>
     <t>Predicted X</t>
   </si>
   <si>
@@ -94,14 +102,103 @@
   </si>
   <si>
     <t>(Angle was reduced to 0 to make sure motion was straight)</t>
+  </si>
+  <si>
+    <t>PROCEEDURE FOR MEASURING ANGLE:</t>
+  </si>
+  <si>
+    <t>Line up protractor center with camera center</t>
+  </si>
+  <si>
+    <t>Line up string with dot</t>
+  </si>
+  <si>
+    <t>read angle</t>
+  </si>
+  <si>
+    <t>Get to position</t>
+  </si>
+  <si>
+    <t>(1-0)</t>
+  </si>
+  <si>
+    <t>Error: &lt;1 degree</t>
+  </si>
+  <si>
+    <t>(tag 2 - 2nd worst tag)</t>
+  </si>
+  <si>
+    <t>X, Y, Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pitch, Range, Yaw</t>
+  </si>
+  <si>
+    <t>0,0 - id1</t>
+  </si>
+  <si>
+    <t>-5.5   23.2    2.6</t>
+  </si>
+  <si>
+    <t>-23.9   -1.4   13.0</t>
+  </si>
+  <si>
+    <t>0,0 - id2</t>
+  </si>
+  <si>
+    <t>0.6   24.7    2.7</t>
+  </si>
+  <si>
+    <t>-24.4   -0.9   13.3</t>
+  </si>
+  <si>
+    <t>0,0 - id3</t>
+  </si>
+  <si>
+    <t>6.5   26.1    2.8</t>
+  </si>
+  <si>
+    <t>-23.5   -0.4   13.8</t>
+  </si>
+  <si>
+    <t>"2,0 - id1"</t>
+  </si>
+  <si>
+    <t>ID pos Data</t>
+  </si>
+  <si>
+    <t>ID error Data</t>
+  </si>
+  <si>
+    <t>"0-0"</t>
+  </si>
+  <si>
+    <t>"2-0"</t>
+  </si>
+  <si>
+    <t>"4-0"</t>
+  </si>
+  <si>
+    <t>"6-0"</t>
+  </si>
+  <si>
+    <t>Measured angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,6 +216,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +250,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,27 +590,27 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>-0.63</v>
@@ -519,7 +633,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>-0.64</v>
@@ -542,7 +656,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>-0.89</v>
@@ -565,7 +679,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>-1.1000000000000001</v>
@@ -588,7 +702,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>-1.18</v>
@@ -611,7 +725,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>-0.85</v>
@@ -634,7 +748,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>0.32</v>
@@ -657,7 +771,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>0.08</v>
@@ -680,7 +794,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>0.23</v>
@@ -703,7 +817,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
         <v>-0.17</v>
@@ -726,26 +840,26 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C035F4D3-A8E7-D347-BA84-866C9ADA4DD1}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,32 +868,248 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24.92</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>24.73</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF0621D-04EA-3A46-98CF-E45D543691ED}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1CC266-47CF-7743-B677-4F2676033337}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
       <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H2">
-        <v>6</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested with 1 camera (multi camera opmode unreliable)
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
+++ b/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE7F138-709A-844E-BEA2-0C2025F8793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DBBCB4-7D00-D344-B9AB-EFF59E719483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
   </bookViews>
   <sheets>
     <sheet name="id1 - Straight On (Angle Cxled)" sheetId="1" r:id="rId1"/>
     <sheet name="id2 - Pointing" sheetId="2" r:id="rId2"/>
     <sheet name="ALLid - Const. Angle" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Location</t>
   </si>
@@ -575,7 +576,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +860,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1CC266-47CF-7743-B677-4F2676033337}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,4 +1116,272 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D282E96-C7C8-384C-B7BF-4C5C0447E2DB}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>-0.63</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5.84</v>
+      </c>
+      <c r="F2" s="1">
+        <v>23.92</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.64</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5.94</v>
+      </c>
+      <c r="F3">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.89</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="F5" s="1">
+        <v>18.27</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1.18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="F6" s="1">
+        <v>16.510000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.85</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="F7" s="1">
+        <v>14.58</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>12.57</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10.66</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8.66</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-0.17</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6.53</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored AprilTagOmeter_TagCentricToFieldCentric to convert tag-centric coords to field-centric coords.
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
+++ b/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5992489-134E-0245-B907-8643E8350527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40FAF0B-095E-BC44-BF5D-723B50BB3103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>Location</t>
   </si>
@@ -209,7 +209,10 @@
     <t>(</t>
   </si>
   <si>
-    <t xml:space="preserve">(if angle = </t>
+    <t>anomaly found: allow all apriltags, pick best, if angle between 0 and 2 degrees, consider calculating difference in X</t>
+  </si>
+  <si>
+    <t>pointing at AprilTag - most accurate</t>
   </si>
 </sst>
 </file>
@@ -1422,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138BC2FA-228B-EE41-9E22-6E75175FADA0}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1530,6 +1533,11 @@
     <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This adds working field coordinates that are at least relatively accurate.
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
+++ b/AprilTag Performance Evaluation/22-3-24 AprilTag Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40FAF0B-095E-BC44-BF5D-723B50BB3103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C8CD5D-E782-5445-9C46-D2B75A7FBE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="7" xr2:uid="{C92DD158-3579-9143-A106-0547BD8B3C6D}"/>
   </bookViews>
   <sheets>
     <sheet name="id1 - Straight On (Angle Cxled)" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="id2 - Pointing, Field Coords" sheetId="5" r:id="rId5"/>
     <sheet name="id2 - straight on" sheetId="6" r:id="rId6"/>
     <sheet name="id2 - subtraction" sheetId="7" r:id="rId7"/>
+    <sheet name="id2 - field coords." sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -290,14 +291,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -318,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +358,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1085,7 +1085,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138BC2FA-228B-EE41-9E22-6E75175FADA0}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1555,127 +1555,139 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="7"/>
-    <col min="4" max="4" width="20.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="3" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="20.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>-0.26</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>0.37</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>23.9</v>
       </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>0.18</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>16.399999999999999</v>
       </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
         <v>16.25</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>-0.65</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>0.45</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>10.7</v>
       </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
         <v>10.5</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="1">
         <v>-1.18</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>0.51</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>6.62</v>
       </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
         <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE73E62-56D8-FF4B-A439-052401C51BE9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>